<commit_message>
Inserindo as diferenças te tempo nas funções, mas meio perdido
</commit_message>
<xml_diff>
--- a/data/EXCEL_populacional/populacional_PBC.xlsx
+++ b/data/EXCEL_populacional/populacional_PBC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Google Drive\IPeC\PBC\PESQUISAS\Scripts\EXCEL_foto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\PBC\R para PBC\pbc\data\EXCEL_populacional\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Saidas" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -460,9 +460,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -480,6 +477,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3251,8 +3257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3345,25 +3351,21 @@
       <c r="H2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="21">
         <v>6</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21">
         <v>0</v>
       </c>
-      <c r="K2" s="8">
+      <c r="M2" s="21">
+        <v>3</v>
+      </c>
+      <c r="N2" s="21">
         <v>0</v>
       </c>
-      <c r="L2" s="8">
-        <v>0</v>
-      </c>
-      <c r="M2" s="8">
-        <v>3</v>
-      </c>
-      <c r="N2" s="8">
-        <v>0</v>
-      </c>
-      <c r="O2" s="8">
+      <c r="O2" s="21">
         <v>3</v>
       </c>
       <c r="P2" s="2" t="s">
@@ -3391,25 +3393,23 @@
       <c r="H3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="8">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8">
+      <c r="I3" s="21"/>
+      <c r="J3" s="21">
         <v>6</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="21">
         <v>15</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="21">
         <v>1</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="21">
         <v>2</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="21">
         <v>2</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="21">
         <v>10</v>
       </c>
       <c r="P3" s="2"/>
@@ -3435,25 +3435,21 @@
       <c r="H4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="21">
         <v>4</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21">
         <v>0</v>
       </c>
-      <c r="K4" s="8">
+      <c r="M4" s="21">
         <v>0</v>
       </c>
-      <c r="L4" s="8">
+      <c r="N4" s="21">
         <v>0</v>
       </c>
-      <c r="M4" s="8">
-        <v>0</v>
-      </c>
-      <c r="N4" s="8">
-        <v>0</v>
-      </c>
-      <c r="O4" s="8">
+      <c r="O4" s="21">
         <v>4</v>
       </c>
       <c r="P4" s="2"/>
@@ -3479,25 +3475,21 @@
       <c r="H5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="21">
         <v>5</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21">
         <v>0</v>
       </c>
-      <c r="K5" s="8">
+      <c r="M5" s="21">
+        <v>2</v>
+      </c>
+      <c r="N5" s="21">
         <v>0</v>
       </c>
-      <c r="L5" s="8">
-        <v>0</v>
-      </c>
-      <c r="M5" s="8">
-        <v>2</v>
-      </c>
-      <c r="N5" s="8">
-        <v>0</v>
-      </c>
-      <c r="O5" s="8">
+      <c r="O5" s="21">
         <v>3</v>
       </c>
       <c r="P5" s="2"/>
@@ -3523,25 +3515,21 @@
       <c r="H6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="21">
         <v>4</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21">
         <v>0</v>
       </c>
-      <c r="K6" s="8">
+      <c r="M6" s="21">
         <v>0</v>
       </c>
-      <c r="L6" s="8">
+      <c r="N6" s="21">
         <v>0</v>
       </c>
-      <c r="M6" s="8">
-        <v>0</v>
-      </c>
-      <c r="N6" s="8">
-        <v>0</v>
-      </c>
-      <c r="O6" s="8">
+      <c r="O6" s="21">
         <v>4</v>
       </c>
       <c r="P6" s="2"/>
@@ -3567,25 +3555,21 @@
       <c r="H7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="21">
         <v>5</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21">
         <v>0</v>
       </c>
-      <c r="K7" s="8">
+      <c r="M7" s="21">
         <v>0</v>
       </c>
-      <c r="L7" s="8">
+      <c r="N7" s="21">
         <v>0</v>
       </c>
-      <c r="M7" s="8">
-        <v>0</v>
-      </c>
-      <c r="N7" s="8">
-        <v>0</v>
-      </c>
-      <c r="O7" s="8">
+      <c r="O7" s="21">
         <v>5</v>
       </c>
       <c r="P7" s="2"/>
@@ -3611,25 +3595,21 @@
       <c r="H8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="21">
         <v>4</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21">
         <v>0</v>
       </c>
-      <c r="K8" s="8">
+      <c r="M8" s="21">
         <v>0</v>
       </c>
-      <c r="L8" s="8">
+      <c r="N8" s="21">
         <v>0</v>
       </c>
-      <c r="M8" s="8">
-        <v>0</v>
-      </c>
-      <c r="N8" s="8">
-        <v>0</v>
-      </c>
-      <c r="O8" s="8">
+      <c r="O8" s="21">
         <v>4</v>
       </c>
       <c r="P8" s="2"/>
@@ -3654,25 +3634,21 @@
       <c r="H9" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="21">
         <v>3</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21">
         <v>0</v>
       </c>
-      <c r="K9" s="8">
+      <c r="M9" s="21">
         <v>0</v>
       </c>
-      <c r="L9" s="8">
+      <c r="N9" s="21">
         <v>0</v>
       </c>
-      <c r="M9" s="8">
-        <v>0</v>
-      </c>
-      <c r="N9" s="8">
-        <v>0</v>
-      </c>
-      <c r="O9" s="8">
+      <c r="O9" s="21">
         <v>3</v>
       </c>
     </row>
@@ -3696,25 +3672,21 @@
       <c r="H10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="21">
         <v>3</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21">
         <v>0</v>
       </c>
-      <c r="K10" s="8">
+      <c r="M10" s="21">
+        <v>1</v>
+      </c>
+      <c r="N10" s="21">
         <v>0</v>
       </c>
-      <c r="L10" s="8">
-        <v>0</v>
-      </c>
-      <c r="M10" s="8">
-        <v>1</v>
-      </c>
-      <c r="N10" s="8">
-        <v>0</v>
-      </c>
-      <c r="O10" s="8">
+      <c r="O10" s="21">
         <v>2</v>
       </c>
     </row>
@@ -3738,25 +3710,21 @@
       <c r="H11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="21">
         <v>4</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21">
         <v>0</v>
       </c>
-      <c r="K11" s="8">
+      <c r="M11" s="21">
+        <v>2</v>
+      </c>
+      <c r="N11" s="21">
         <v>0</v>
       </c>
-      <c r="L11" s="8">
-        <v>0</v>
-      </c>
-      <c r="M11" s="8">
-        <v>2</v>
-      </c>
-      <c r="N11" s="8">
-        <v>0</v>
-      </c>
-      <c r="O11" s="8">
+      <c r="O11" s="21">
         <v>2</v>
       </c>
     </row>
@@ -3780,25 +3748,21 @@
       <c r="H12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="21">
         <v>7</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21">
         <v>0</v>
       </c>
-      <c r="K12" s="8">
+      <c r="M12" s="21">
+        <v>3</v>
+      </c>
+      <c r="N12" s="21">
         <v>0</v>
       </c>
-      <c r="L12" s="8">
-        <v>0</v>
-      </c>
-      <c r="M12" s="8">
-        <v>3</v>
-      </c>
-      <c r="N12" s="8">
-        <v>0</v>
-      </c>
-      <c r="O12" s="8">
+      <c r="O12" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3822,25 +3786,21 @@
       <c r="H13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="21">
         <v>4</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21">
         <v>0</v>
       </c>
-      <c r="K13" s="8">
+      <c r="M13" s="21">
         <v>0</v>
       </c>
-      <c r="L13" s="8">
+      <c r="N13" s="21">
         <v>0</v>
       </c>
-      <c r="M13" s="8">
-        <v>0</v>
-      </c>
-      <c r="N13" s="8">
-        <v>0</v>
-      </c>
-      <c r="O13" s="8">
+      <c r="O13" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3864,25 +3824,21 @@
       <c r="H14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="21">
         <v>5</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21">
         <v>0</v>
       </c>
-      <c r="K14" s="8">
+      <c r="M14" s="21">
+        <v>2</v>
+      </c>
+      <c r="N14" s="21">
         <v>0</v>
       </c>
-      <c r="L14" s="8">
-        <v>0</v>
-      </c>
-      <c r="M14" s="8">
-        <v>2</v>
-      </c>
-      <c r="N14" s="8">
-        <v>0</v>
-      </c>
-      <c r="O14" s="8">
+      <c r="O14" s="21">
         <v>3</v>
       </c>
     </row>
@@ -3906,25 +3862,23 @@
       <c r="H15" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="21"/>
+      <c r="J15" s="21">
+        <v>10</v>
+      </c>
+      <c r="K15" s="21">
+        <v>12</v>
+      </c>
+      <c r="L15" s="21">
         <v>0</v>
       </c>
-      <c r="J15" s="8">
-        <v>10</v>
-      </c>
-      <c r="K15" s="8">
-        <v>12</v>
-      </c>
-      <c r="L15" s="8">
+      <c r="M15" s="21">
         <v>0</v>
       </c>
-      <c r="M15" s="8">
-        <v>0</v>
-      </c>
-      <c r="N15" s="8">
+      <c r="N15" s="21">
         <v>4</v>
       </c>
-      <c r="O15" s="8">
+      <c r="O15" s="21">
         <v>8</v>
       </c>
     </row>
@@ -3948,25 +3902,21 @@
       <c r="H16" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="22">
         <v>3</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="21">
         <v>0</v>
       </c>
-      <c r="K16" s="14">
+      <c r="M16" s="23">
+        <v>1</v>
+      </c>
+      <c r="N16" s="23">
         <v>0</v>
       </c>
-      <c r="L16" s="8">
-        <v>0</v>
-      </c>
-      <c r="M16" s="10">
-        <v>1</v>
-      </c>
-      <c r="N16" s="10">
-        <v>0</v>
-      </c>
-      <c r="O16" s="10">
+      <c r="O16" s="23">
         <v>2</v>
       </c>
     </row>
@@ -3990,25 +3940,21 @@
       <c r="H17" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="22">
         <v>3</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="21">
         <v>0</v>
       </c>
-      <c r="K17" s="14">
+      <c r="M17" s="23">
         <v>0</v>
       </c>
-      <c r="L17" s="8">
+      <c r="N17" s="23">
         <v>0</v>
       </c>
-      <c r="M17" s="10">
-        <v>0</v>
-      </c>
-      <c r="N17" s="10">
-        <v>0</v>
-      </c>
-      <c r="O17" s="10">
+      <c r="O17" s="23">
         <v>3</v>
       </c>
     </row>
@@ -4032,28 +3978,24 @@
       <c r="H18" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="22">
         <v>7</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="21">
         <v>0</v>
       </c>
-      <c r="K18" s="14">
+      <c r="M18" s="23">
+        <v>1</v>
+      </c>
+      <c r="N18" s="23">
         <v>0</v>
       </c>
-      <c r="L18" s="8">
-        <v>0</v>
-      </c>
-      <c r="M18" s="10">
-        <v>1</v>
-      </c>
-      <c r="N18" s="10">
-        <v>0</v>
-      </c>
-      <c r="O18" s="10">
+      <c r="O18" s="23">
         <v>6</v>
       </c>
-      <c r="P18" s="15" t="s">
+      <c r="P18" s="14" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4077,25 +4019,21 @@
       <c r="H19" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="22">
         <v>4</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="21">
         <v>0</v>
       </c>
-      <c r="K19" s="14">
+      <c r="M19" s="23">
+        <v>1</v>
+      </c>
+      <c r="N19" s="23">
         <v>0</v>
       </c>
-      <c r="L19" s="8">
-        <v>0</v>
-      </c>
-      <c r="M19" s="10">
-        <v>1</v>
-      </c>
-      <c r="N19" s="10">
-        <v>0</v>
-      </c>
-      <c r="O19" s="10">
+      <c r="O19" s="23">
         <v>3</v>
       </c>
     </row>
@@ -4119,25 +4057,21 @@
       <c r="H20" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="22">
         <v>2</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="21">
         <v>0</v>
       </c>
-      <c r="K20" s="14">
+      <c r="M20" s="23">
         <v>0</v>
       </c>
-      <c r="L20" s="8">
+      <c r="N20" s="23">
         <v>0</v>
       </c>
-      <c r="M20" s="10">
-        <v>0</v>
-      </c>
-      <c r="N20" s="10">
-        <v>0</v>
-      </c>
-      <c r="O20" s="10">
+      <c r="O20" s="23">
         <v>2</v>
       </c>
     </row>
@@ -4161,25 +4095,21 @@
       <c r="H21" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="22">
         <v>4</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="21">
         <v>0</v>
       </c>
-      <c r="K21" s="14">
+      <c r="M21" s="23">
         <v>0</v>
       </c>
-      <c r="L21" s="8">
+      <c r="N21" s="23">
         <v>0</v>
       </c>
-      <c r="M21" s="10">
-        <v>0</v>
-      </c>
-      <c r="N21" s="10">
-        <v>0</v>
-      </c>
-      <c r="O21" s="10">
+      <c r="O21" s="23">
         <v>4</v>
       </c>
     </row>
@@ -4203,25 +4133,21 @@
       <c r="H22" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="22">
         <v>4</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="21">
         <v>0</v>
       </c>
-      <c r="K22" s="14">
+      <c r="M22" s="23">
+        <v>1</v>
+      </c>
+      <c r="N22" s="23">
         <v>0</v>
       </c>
-      <c r="L22" s="8">
-        <v>0</v>
-      </c>
-      <c r="M22" s="10">
-        <v>1</v>
-      </c>
-      <c r="N22" s="10">
-        <v>0</v>
-      </c>
-      <c r="O22" s="10">
+      <c r="O22" s="23">
         <v>3</v>
       </c>
     </row>
@@ -4245,28 +4171,24 @@
       <c r="H23" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I23" s="14">
+      <c r="I23" s="22">
         <v>10</v>
       </c>
-      <c r="J23" s="14">
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="21">
         <v>0</v>
       </c>
-      <c r="K23" s="14">
+      <c r="M23" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="N23" s="23">
         <v>0</v>
       </c>
-      <c r="L23" s="8">
-        <v>0</v>
-      </c>
-      <c r="M23" s="14" t="s">
+      <c r="O23" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="N23" s="10">
-        <v>0</v>
-      </c>
-      <c r="O23" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="P23" s="15" t="s">
+      <c r="P23" s="14" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4290,25 +4212,21 @@
       <c r="H24" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="22">
         <v>3</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="21">
         <v>0</v>
       </c>
-      <c r="K24" s="14">
+      <c r="M24" s="23">
         <v>0</v>
       </c>
-      <c r="L24" s="8">
+      <c r="N24" s="23">
         <v>0</v>
       </c>
-      <c r="M24" s="10">
-        <v>0</v>
-      </c>
-      <c r="N24" s="10">
-        <v>0</v>
-      </c>
-      <c r="O24" s="10">
+      <c r="O24" s="23">
         <v>3</v>
       </c>
     </row>
@@ -4332,25 +4250,21 @@
       <c r="H25" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I25" s="14">
+      <c r="I25" s="22">
         <v>4</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="21">
         <v>0</v>
       </c>
-      <c r="K25" s="14">
+      <c r="M25" s="23">
+        <v>1</v>
+      </c>
+      <c r="N25" s="23">
         <v>0</v>
       </c>
-      <c r="L25" s="8">
-        <v>0</v>
-      </c>
-      <c r="M25" s="10">
-        <v>1</v>
-      </c>
-      <c r="N25" s="10">
-        <v>0</v>
-      </c>
-      <c r="O25" s="10">
+      <c r="O25" s="23">
         <v>3</v>
       </c>
     </row>
@@ -4374,25 +4288,21 @@
       <c r="H26" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I26" s="14">
+      <c r="I26" s="22">
         <v>3</v>
       </c>
-      <c r="J26" s="14">
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="21">
         <v>0</v>
       </c>
-      <c r="K26" s="14">
+      <c r="M26" s="23">
+        <v>1</v>
+      </c>
+      <c r="N26" s="23">
         <v>0</v>
       </c>
-      <c r="L26" s="8">
-        <v>0</v>
-      </c>
-      <c r="M26" s="10">
-        <v>1</v>
-      </c>
-      <c r="N26" s="10">
-        <v>0</v>
-      </c>
-      <c r="O26" s="10">
+      <c r="O26" s="23">
         <v>2</v>
       </c>
     </row>
@@ -11224,7 +11134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -11244,328 +11154,328 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20">
         <v>-47.920033333333301</v>
       </c>
-      <c r="I2" s="21">
+      <c r="I2" s="20">
         <v>-25.051391666666699</v>
       </c>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21" t="s">
+      <c r="J2" s="20"/>
+      <c r="K2" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="20" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20">
         <v>-47.931680555555602</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="20">
         <v>-25.062586111111099</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21" t="s">
+      <c r="J3" s="20"/>
+      <c r="K3" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="20" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20">
         <v>-47.899380555555602</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="20">
         <v>-24.998758333333299</v>
       </c>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21" t="s">
+      <c r="J4" s="20"/>
+      <c r="K4" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="20" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20">
         <v>-47.898344444444398</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="20">
         <v>-24.994969444444401</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21" t="s">
+      <c r="J5" s="20"/>
+      <c r="K5" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="L5" s="20" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21">
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20">
         <v>-47.9110444444444</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="20">
         <v>-25.057277777777799</v>
       </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21" t="s">
+      <c r="J6" s="20"/>
+      <c r="K6" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="L6" s="20" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21">
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20">
         <v>-47.910422222222202</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="20">
         <v>-25.057700000000001</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21" t="s">
+      <c r="J7" s="20"/>
+      <c r="K7" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="L7" s="20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21">
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20">
         <v>-47.909077777777803</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="20">
         <v>-25.059052777777801</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21" t="s">
+      <c r="J8" s="20"/>
+      <c r="K8" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21">
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20">
         <v>-47.908280555555599</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="20">
         <v>-25.0588388888889</v>
       </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21" t="s">
+      <c r="J9" s="20"/>
+      <c r="K9" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="L9" s="21" t="s">
+      <c r="L9" s="20" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21">
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20">
         <v>-47.908983333333303</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="20">
         <v>-25.0589166666667</v>
       </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21" t="s">
+      <c r="J10" s="20"/>
+      <c r="K10" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="L10" s="20" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20">
         <v>-47.909352777777798</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="20">
         <v>-25.056602777777801</v>
       </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21" t="s">
+      <c r="J11" s="20"/>
+      <c r="K11" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="L11" s="21" t="s">
+      <c r="L11" s="20" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20">
         <v>-47.894733333333299</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="20">
         <v>-25.057719444444398</v>
       </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21" t="s">
+      <c r="J12" s="20"/>
+      <c r="K12" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="L12" s="21" t="s">
+      <c r="L12" s="20" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20">
         <v>-47.927783333333302</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="20">
         <v>-25.064827777777801</v>
       </c>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21" t="s">
+      <c r="J13" s="20"/>
+      <c r="K13" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="L13" s="21" t="s">
+      <c r="L13" s="20" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel com NAs nos tamanhos de grupo
</commit_message>
<xml_diff>
--- a/data/EXCEL_populacional/populacional_PBC.xlsx
+++ b/data/EXCEL_populacional/populacional_PBC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Google Drive\IPeC\PBC\PESQUISAS\Scripts\EXCEL_foto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\PBC\R para PBC\pbc\data\EXCEL_populacional\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Saidas" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -460,9 +460,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -480,6 +477,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3251,8 +3257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3345,25 +3351,21 @@
       <c r="H2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="21">
         <v>6</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21">
         <v>0</v>
       </c>
-      <c r="K2" s="8">
+      <c r="M2" s="21">
+        <v>3</v>
+      </c>
+      <c r="N2" s="21">
         <v>0</v>
       </c>
-      <c r="L2" s="8">
-        <v>0</v>
-      </c>
-      <c r="M2" s="8">
-        <v>3</v>
-      </c>
-      <c r="N2" s="8">
-        <v>0</v>
-      </c>
-      <c r="O2" s="8">
+      <c r="O2" s="21">
         <v>3</v>
       </c>
       <c r="P2" s="2" t="s">
@@ -3391,25 +3393,23 @@
       <c r="H3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="8">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8">
+      <c r="I3" s="21"/>
+      <c r="J3" s="21">
         <v>6</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="21">
         <v>15</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="21">
         <v>1</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="21">
         <v>2</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="21">
         <v>2</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="21">
         <v>10</v>
       </c>
       <c r="P3" s="2"/>
@@ -3435,25 +3435,21 @@
       <c r="H4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="21">
         <v>4</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21">
         <v>0</v>
       </c>
-      <c r="K4" s="8">
+      <c r="M4" s="21">
         <v>0</v>
       </c>
-      <c r="L4" s="8">
+      <c r="N4" s="21">
         <v>0</v>
       </c>
-      <c r="M4" s="8">
-        <v>0</v>
-      </c>
-      <c r="N4" s="8">
-        <v>0</v>
-      </c>
-      <c r="O4" s="8">
+      <c r="O4" s="21">
         <v>4</v>
       </c>
       <c r="P4" s="2"/>
@@ -3479,25 +3475,21 @@
       <c r="H5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="21">
         <v>5</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21">
         <v>0</v>
       </c>
-      <c r="K5" s="8">
+      <c r="M5" s="21">
+        <v>2</v>
+      </c>
+      <c r="N5" s="21">
         <v>0</v>
       </c>
-      <c r="L5" s="8">
-        <v>0</v>
-      </c>
-      <c r="M5" s="8">
-        <v>2</v>
-      </c>
-      <c r="N5" s="8">
-        <v>0</v>
-      </c>
-      <c r="O5" s="8">
+      <c r="O5" s="21">
         <v>3</v>
       </c>
       <c r="P5" s="2"/>
@@ -3523,25 +3515,21 @@
       <c r="H6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="21">
         <v>4</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21">
         <v>0</v>
       </c>
-      <c r="K6" s="8">
+      <c r="M6" s="21">
         <v>0</v>
       </c>
-      <c r="L6" s="8">
+      <c r="N6" s="21">
         <v>0</v>
       </c>
-      <c r="M6" s="8">
-        <v>0</v>
-      </c>
-      <c r="N6" s="8">
-        <v>0</v>
-      </c>
-      <c r="O6" s="8">
+      <c r="O6" s="21">
         <v>4</v>
       </c>
       <c r="P6" s="2"/>
@@ -3567,25 +3555,21 @@
       <c r="H7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="21">
         <v>5</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21">
         <v>0</v>
       </c>
-      <c r="K7" s="8">
+      <c r="M7" s="21">
         <v>0</v>
       </c>
-      <c r="L7" s="8">
+      <c r="N7" s="21">
         <v>0</v>
       </c>
-      <c r="M7" s="8">
-        <v>0</v>
-      </c>
-      <c r="N7" s="8">
-        <v>0</v>
-      </c>
-      <c r="O7" s="8">
+      <c r="O7" s="21">
         <v>5</v>
       </c>
       <c r="P7" s="2"/>
@@ -3611,25 +3595,21 @@
       <c r="H8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="21">
         <v>4</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21">
         <v>0</v>
       </c>
-      <c r="K8" s="8">
+      <c r="M8" s="21">
         <v>0</v>
       </c>
-      <c r="L8" s="8">
+      <c r="N8" s="21">
         <v>0</v>
       </c>
-      <c r="M8" s="8">
-        <v>0</v>
-      </c>
-      <c r="N8" s="8">
-        <v>0</v>
-      </c>
-      <c r="O8" s="8">
+      <c r="O8" s="21">
         <v>4</v>
       </c>
       <c r="P8" s="2"/>
@@ -3654,25 +3634,21 @@
       <c r="H9" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="21">
         <v>3</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21">
         <v>0</v>
       </c>
-      <c r="K9" s="8">
+      <c r="M9" s="21">
         <v>0</v>
       </c>
-      <c r="L9" s="8">
+      <c r="N9" s="21">
         <v>0</v>
       </c>
-      <c r="M9" s="8">
-        <v>0</v>
-      </c>
-      <c r="N9" s="8">
-        <v>0</v>
-      </c>
-      <c r="O9" s="8">
+      <c r="O9" s="21">
         <v>3</v>
       </c>
     </row>
@@ -3696,25 +3672,21 @@
       <c r="H10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="21">
         <v>3</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21">
         <v>0</v>
       </c>
-      <c r="K10" s="8">
+      <c r="M10" s="21">
+        <v>1</v>
+      </c>
+      <c r="N10" s="21">
         <v>0</v>
       </c>
-      <c r="L10" s="8">
-        <v>0</v>
-      </c>
-      <c r="M10" s="8">
-        <v>1</v>
-      </c>
-      <c r="N10" s="8">
-        <v>0</v>
-      </c>
-      <c r="O10" s="8">
+      <c r="O10" s="21">
         <v>2</v>
       </c>
     </row>
@@ -3738,25 +3710,21 @@
       <c r="H11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="21">
         <v>4</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21">
         <v>0</v>
       </c>
-      <c r="K11" s="8">
+      <c r="M11" s="21">
+        <v>2</v>
+      </c>
+      <c r="N11" s="21">
         <v>0</v>
       </c>
-      <c r="L11" s="8">
-        <v>0</v>
-      </c>
-      <c r="M11" s="8">
-        <v>2</v>
-      </c>
-      <c r="N11" s="8">
-        <v>0</v>
-      </c>
-      <c r="O11" s="8">
+      <c r="O11" s="21">
         <v>2</v>
       </c>
     </row>
@@ -3780,25 +3748,21 @@
       <c r="H12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="21">
         <v>7</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21">
         <v>0</v>
       </c>
-      <c r="K12" s="8">
+      <c r="M12" s="21">
+        <v>3</v>
+      </c>
+      <c r="N12" s="21">
         <v>0</v>
       </c>
-      <c r="L12" s="8">
-        <v>0</v>
-      </c>
-      <c r="M12" s="8">
-        <v>3</v>
-      </c>
-      <c r="N12" s="8">
-        <v>0</v>
-      </c>
-      <c r="O12" s="8">
+      <c r="O12" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3822,25 +3786,21 @@
       <c r="H13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="21">
         <v>4</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21">
         <v>0</v>
       </c>
-      <c r="K13" s="8">
+      <c r="M13" s="21">
         <v>0</v>
       </c>
-      <c r="L13" s="8">
+      <c r="N13" s="21">
         <v>0</v>
       </c>
-      <c r="M13" s="8">
-        <v>0</v>
-      </c>
-      <c r="N13" s="8">
-        <v>0</v>
-      </c>
-      <c r="O13" s="8">
+      <c r="O13" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3864,25 +3824,21 @@
       <c r="H14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="21">
         <v>5</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21">
         <v>0</v>
       </c>
-      <c r="K14" s="8">
+      <c r="M14" s="21">
+        <v>2</v>
+      </c>
+      <c r="N14" s="21">
         <v>0</v>
       </c>
-      <c r="L14" s="8">
-        <v>0</v>
-      </c>
-      <c r="M14" s="8">
-        <v>2</v>
-      </c>
-      <c r="N14" s="8">
-        <v>0</v>
-      </c>
-      <c r="O14" s="8">
+      <c r="O14" s="21">
         <v>3</v>
       </c>
     </row>
@@ -3906,25 +3862,23 @@
       <c r="H15" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="21"/>
+      <c r="J15" s="21">
+        <v>10</v>
+      </c>
+      <c r="K15" s="21">
+        <v>12</v>
+      </c>
+      <c r="L15" s="21">
         <v>0</v>
       </c>
-      <c r="J15" s="8">
-        <v>10</v>
-      </c>
-      <c r="K15" s="8">
-        <v>12</v>
-      </c>
-      <c r="L15" s="8">
+      <c r="M15" s="21">
         <v>0</v>
       </c>
-      <c r="M15" s="8">
-        <v>0</v>
-      </c>
-      <c r="N15" s="8">
+      <c r="N15" s="21">
         <v>4</v>
       </c>
-      <c r="O15" s="8">
+      <c r="O15" s="21">
         <v>8</v>
       </c>
     </row>
@@ -3948,25 +3902,21 @@
       <c r="H16" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="22">
         <v>3</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="21">
         <v>0</v>
       </c>
-      <c r="K16" s="14">
+      <c r="M16" s="23">
+        <v>1</v>
+      </c>
+      <c r="N16" s="23">
         <v>0</v>
       </c>
-      <c r="L16" s="8">
-        <v>0</v>
-      </c>
-      <c r="M16" s="10">
-        <v>1</v>
-      </c>
-      <c r="N16" s="10">
-        <v>0</v>
-      </c>
-      <c r="O16" s="10">
+      <c r="O16" s="23">
         <v>2</v>
       </c>
     </row>
@@ -3990,25 +3940,21 @@
       <c r="H17" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="22">
         <v>3</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="21">
         <v>0</v>
       </c>
-      <c r="K17" s="14">
+      <c r="M17" s="23">
         <v>0</v>
       </c>
-      <c r="L17" s="8">
+      <c r="N17" s="23">
         <v>0</v>
       </c>
-      <c r="M17" s="10">
-        <v>0</v>
-      </c>
-      <c r="N17" s="10">
-        <v>0</v>
-      </c>
-      <c r="O17" s="10">
+      <c r="O17" s="23">
         <v>3</v>
       </c>
     </row>
@@ -4032,28 +3978,24 @@
       <c r="H18" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="22">
         <v>7</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="21">
         <v>0</v>
       </c>
-      <c r="K18" s="14">
+      <c r="M18" s="23">
+        <v>1</v>
+      </c>
+      <c r="N18" s="23">
         <v>0</v>
       </c>
-      <c r="L18" s="8">
-        <v>0</v>
-      </c>
-      <c r="M18" s="10">
-        <v>1</v>
-      </c>
-      <c r="N18" s="10">
-        <v>0</v>
-      </c>
-      <c r="O18" s="10">
+      <c r="O18" s="23">
         <v>6</v>
       </c>
-      <c r="P18" s="15" t="s">
+      <c r="P18" s="14" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4077,25 +4019,21 @@
       <c r="H19" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="22">
         <v>4</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="21">
         <v>0</v>
       </c>
-      <c r="K19" s="14">
+      <c r="M19" s="23">
+        <v>1</v>
+      </c>
+      <c r="N19" s="23">
         <v>0</v>
       </c>
-      <c r="L19" s="8">
-        <v>0</v>
-      </c>
-      <c r="M19" s="10">
-        <v>1</v>
-      </c>
-      <c r="N19" s="10">
-        <v>0</v>
-      </c>
-      <c r="O19" s="10">
+      <c r="O19" s="23">
         <v>3</v>
       </c>
     </row>
@@ -4119,25 +4057,21 @@
       <c r="H20" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="22">
         <v>2</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="21">
         <v>0</v>
       </c>
-      <c r="K20" s="14">
+      <c r="M20" s="23">
         <v>0</v>
       </c>
-      <c r="L20" s="8">
+      <c r="N20" s="23">
         <v>0</v>
       </c>
-      <c r="M20" s="10">
-        <v>0</v>
-      </c>
-      <c r="N20" s="10">
-        <v>0</v>
-      </c>
-      <c r="O20" s="10">
+      <c r="O20" s="23">
         <v>2</v>
       </c>
     </row>
@@ -4161,25 +4095,21 @@
       <c r="H21" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="22">
         <v>4</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="21">
         <v>0</v>
       </c>
-      <c r="K21" s="14">
+      <c r="M21" s="23">
         <v>0</v>
       </c>
-      <c r="L21" s="8">
+      <c r="N21" s="23">
         <v>0</v>
       </c>
-      <c r="M21" s="10">
-        <v>0</v>
-      </c>
-      <c r="N21" s="10">
-        <v>0</v>
-      </c>
-      <c r="O21" s="10">
+      <c r="O21" s="23">
         <v>4</v>
       </c>
     </row>
@@ -4203,25 +4133,21 @@
       <c r="H22" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="22">
         <v>4</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="21">
         <v>0</v>
       </c>
-      <c r="K22" s="14">
+      <c r="M22" s="23">
+        <v>1</v>
+      </c>
+      <c r="N22" s="23">
         <v>0</v>
       </c>
-      <c r="L22" s="8">
-        <v>0</v>
-      </c>
-      <c r="M22" s="10">
-        <v>1</v>
-      </c>
-      <c r="N22" s="10">
-        <v>0</v>
-      </c>
-      <c r="O22" s="10">
+      <c r="O22" s="23">
         <v>3</v>
       </c>
     </row>
@@ -4245,28 +4171,24 @@
       <c r="H23" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I23" s="14">
+      <c r="I23" s="22">
         <v>10</v>
       </c>
-      <c r="J23" s="14">
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="21">
         <v>0</v>
       </c>
-      <c r="K23" s="14">
+      <c r="M23" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="N23" s="23">
         <v>0</v>
       </c>
-      <c r="L23" s="8">
-        <v>0</v>
-      </c>
-      <c r="M23" s="14" t="s">
+      <c r="O23" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="N23" s="10">
-        <v>0</v>
-      </c>
-      <c r="O23" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="P23" s="15" t="s">
+      <c r="P23" s="14" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4290,25 +4212,21 @@
       <c r="H24" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="22">
         <v>3</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="21">
         <v>0</v>
       </c>
-      <c r="K24" s="14">
+      <c r="M24" s="23">
         <v>0</v>
       </c>
-      <c r="L24" s="8">
+      <c r="N24" s="23">
         <v>0</v>
       </c>
-      <c r="M24" s="10">
-        <v>0</v>
-      </c>
-      <c r="N24" s="10">
-        <v>0</v>
-      </c>
-      <c r="O24" s="10">
+      <c r="O24" s="23">
         <v>3</v>
       </c>
     </row>
@@ -4332,25 +4250,21 @@
       <c r="H25" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="I25" s="14">
+      <c r="I25" s="22">
         <v>4</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="21">
         <v>0</v>
       </c>
-      <c r="K25" s="14">
+      <c r="M25" s="23">
+        <v>1</v>
+      </c>
+      <c r="N25" s="23">
         <v>0</v>
       </c>
-      <c r="L25" s="8">
-        <v>0</v>
-      </c>
-      <c r="M25" s="10">
-        <v>1</v>
-      </c>
-      <c r="N25" s="10">
-        <v>0</v>
-      </c>
-      <c r="O25" s="10">
+      <c r="O25" s="23">
         <v>3</v>
       </c>
     </row>
@@ -4374,25 +4288,21 @@
       <c r="H26" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I26" s="14">
+      <c r="I26" s="22">
         <v>3</v>
       </c>
-      <c r="J26" s="14">
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="21">
         <v>0</v>
       </c>
-      <c r="K26" s="14">
+      <c r="M26" s="23">
+        <v>1</v>
+      </c>
+      <c r="N26" s="23">
         <v>0</v>
       </c>
-      <c r="L26" s="8">
-        <v>0</v>
-      </c>
-      <c r="M26" s="10">
-        <v>1</v>
-      </c>
-      <c r="N26" s="10">
-        <v>0</v>
-      </c>
-      <c r="O26" s="10">
+      <c r="O26" s="23">
         <v>2</v>
       </c>
     </row>
@@ -11224,7 +11134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -11244,328 +11154,328 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20">
         <v>-47.920033333333301</v>
       </c>
-      <c r="I2" s="21">
+      <c r="I2" s="20">
         <v>-25.051391666666699</v>
       </c>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21" t="s">
+      <c r="J2" s="20"/>
+      <c r="K2" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="20" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20">
         <v>-47.931680555555602</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="20">
         <v>-25.062586111111099</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21" t="s">
+      <c r="J3" s="20"/>
+      <c r="K3" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="20" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20">
         <v>-47.899380555555602</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="20">
         <v>-24.998758333333299</v>
       </c>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21" t="s">
+      <c r="J4" s="20"/>
+      <c r="K4" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="20" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20">
         <v>-47.898344444444398</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="20">
         <v>-24.994969444444401</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21" t="s">
+      <c r="J5" s="20"/>
+      <c r="K5" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="L5" s="20" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21">
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20">
         <v>-47.9110444444444</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="20">
         <v>-25.057277777777799</v>
       </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21" t="s">
+      <c r="J6" s="20"/>
+      <c r="K6" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="L6" s="20" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21">
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20">
         <v>-47.910422222222202</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="20">
         <v>-25.057700000000001</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21" t="s">
+      <c r="J7" s="20"/>
+      <c r="K7" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="L7" s="20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21">
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20">
         <v>-47.909077777777803</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="20">
         <v>-25.059052777777801</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21" t="s">
+      <c r="J8" s="20"/>
+      <c r="K8" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21">
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20">
         <v>-47.908280555555599</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="20">
         <v>-25.0588388888889</v>
       </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21" t="s">
+      <c r="J9" s="20"/>
+      <c r="K9" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="L9" s="21" t="s">
+      <c r="L9" s="20" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21">
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20">
         <v>-47.908983333333303</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="20">
         <v>-25.0589166666667</v>
       </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21" t="s">
+      <c r="J10" s="20"/>
+      <c r="K10" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="L10" s="20" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20">
         <v>-47.909352777777798</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="20">
         <v>-25.056602777777801</v>
       </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21" t="s">
+      <c r="J11" s="20"/>
+      <c r="K11" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="L11" s="21" t="s">
+      <c r="L11" s="20" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20">
         <v>-47.894733333333299</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="20">
         <v>-25.057719444444398</v>
       </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21" t="s">
+      <c r="J12" s="20"/>
+      <c r="K12" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="L12" s="21" t="s">
+      <c r="L12" s="20" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20">
         <v>-47.927783333333302</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="20">
         <v>-25.064827777777801</v>
       </c>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21" t="s">
+      <c r="J13" s="20"/>
+      <c r="K13" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="L13" s="21" t="s">
+      <c r="L13" s="20" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>